<commit_message>
excel related scenario added
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nuclues\IdeaProjects\cucumber-bdd-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2F9B9C-4A28-4C0E-A9AE-12CBA874FA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF26449-7153-4EA3-B2BC-AA131BB65CD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="3150" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FE8D01E6-C1E3-4338-AC3B-B82F2337A162}"/>
+    <workbookView xWindow="2730" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{FE8D01E6-C1E3-4338-AC3B-B82F2337A162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="105">
   <si>
     <t>Execute</t>
   </si>
@@ -91,268 +91,256 @@
     <t>$16.51</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Faded Short Sleeve T-shirts</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>$16.40</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Michaelina</t>
+  </si>
+  <si>
+    <t>Feveryear</t>
+  </si>
+  <si>
+    <t>DcoiTeHjEsB</t>
+  </si>
+  <si>
+    <t>8 Marquette Parkway</t>
+  </si>
+  <si>
+    <t>Abilene</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>325-863-0055</t>
+  </si>
+  <si>
+    <t>Goldi</t>
+  </si>
+  <si>
+    <t>Hearfield</t>
+  </si>
+  <si>
+    <t>5ELQjynv3lw</t>
+  </si>
+  <si>
+    <t>8634 Eastwood Place</t>
+  </si>
+  <si>
+    <t>New Orleans</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>504-864-7349</t>
+  </si>
+  <si>
+    <t>Daisie</t>
+  </si>
+  <si>
+    <t>Spridgeon</t>
+  </si>
+  <si>
+    <t>0ljG5SoBm</t>
+  </si>
+  <si>
+    <t>24674 Forest Park</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>801-340-6765</t>
+  </si>
+  <si>
+    <t>Kliment</t>
+  </si>
+  <si>
+    <t>Huxtable</t>
+  </si>
+  <si>
+    <t>Z7NvpJ7oB1</t>
+  </si>
+  <si>
+    <t>2546 Oriole Center</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>412-529-9524</t>
+  </si>
+  <si>
+    <t>Kerianne</t>
+  </si>
+  <si>
+    <t>Doddemeede</t>
+  </si>
+  <si>
+    <t>rV7NBj</t>
+  </si>
+  <si>
+    <t>3557 Iowa Center</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>251-839-5757</t>
+  </si>
+  <si>
+    <t>Robena</t>
+  </si>
+  <si>
+    <t>Dodshon</t>
+  </si>
+  <si>
+    <t>qUqCn6</t>
+  </si>
+  <si>
+    <t>63 Nova Drive</t>
+  </si>
+  <si>
+    <t>Elmira</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>607-341-1537</t>
+  </si>
+  <si>
+    <t>Rakel</t>
+  </si>
+  <si>
+    <t>Bartot</t>
+  </si>
+  <si>
+    <t>Hh6W5m</t>
+  </si>
+  <si>
+    <t>03 Cambridge Way</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>804-805-8334</t>
+  </si>
+  <si>
+    <t>Casi</t>
+  </si>
+  <si>
+    <t>Terram</t>
+  </si>
+  <si>
+    <t>6KxfV20dnhAI</t>
+  </si>
+  <si>
+    <t>9 Florence Circle</t>
+  </si>
+  <si>
+    <t>Fullerton</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>714-220-2718</t>
+  </si>
+  <si>
+    <t>Erinna</t>
+  </si>
+  <si>
+    <t>Luckhurst</t>
+  </si>
+  <si>
+    <t>gu4QcS9El1Zf</t>
+  </si>
+  <si>
+    <t>6 Dryden Point</t>
+  </si>
+  <si>
+    <t>Tallahassee</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>850-826-7869</t>
+  </si>
+  <si>
+    <t>Darnall</t>
+  </si>
+  <si>
+    <t>Screech</t>
+  </si>
+  <si>
+    <t>zDm8CSBNl</t>
+  </si>
+  <si>
+    <t>16 Oxford Junction</t>
+  </si>
+  <si>
+    <t>504-339-3107</t>
+  </si>
+  <si>
+    <t>$28.98</t>
+  </si>
+  <si>
     <t>$27.00</t>
   </si>
   <si>
-    <t>$26.00</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Faded Short Sleeve T-shirts</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>$16.40</t>
-  </si>
-  <si>
-    <t>$28.99</t>
-  </si>
-  <si>
-    <t>dfs</t>
-  </si>
-  <si>
-    <t>fdsf</t>
-  </si>
-  <si>
-    <t>fdsdf</t>
-  </si>
-  <si>
-    <t>fdsfd</t>
-  </si>
-  <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Street Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Michaelina</t>
-  </si>
-  <si>
-    <t>Feveryear</t>
-  </si>
-  <si>
-    <t>DcoiTeHjEsB</t>
-  </si>
-  <si>
-    <t>8 Marquette Parkway</t>
-  </si>
-  <si>
-    <t>Abilene</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>325-863-0055</t>
-  </si>
-  <si>
-    <t>Goldi</t>
-  </si>
-  <si>
-    <t>Hearfield</t>
-  </si>
-  <si>
-    <t>5ELQjynv3lw</t>
-  </si>
-  <si>
-    <t>8634 Eastwood Place</t>
-  </si>
-  <si>
-    <t>New Orleans</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>504-864-7349</t>
-  </si>
-  <si>
-    <t>Daisie</t>
-  </si>
-  <si>
-    <t>Spridgeon</t>
-  </si>
-  <si>
-    <t>0ljG5SoBm</t>
-  </si>
-  <si>
-    <t>24674 Forest Park</t>
-  </si>
-  <si>
-    <t>Salt Lake City</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>801-340-6765</t>
-  </si>
-  <si>
-    <t>Kliment</t>
-  </si>
-  <si>
-    <t>Huxtable</t>
-  </si>
-  <si>
-    <t>Z7NvpJ7oB1</t>
-  </si>
-  <si>
-    <t>2546 Oriole Center</t>
-  </si>
-  <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>412-529-9524</t>
-  </si>
-  <si>
-    <t>Kerianne</t>
-  </si>
-  <si>
-    <t>Doddemeede</t>
-  </si>
-  <si>
-    <t>rV7NBj</t>
-  </si>
-  <si>
-    <t>3557 Iowa Center</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>251-839-5757</t>
-  </si>
-  <si>
-    <t>Robena</t>
-  </si>
-  <si>
-    <t>Dodshon</t>
-  </si>
-  <si>
-    <t>qUqCn6</t>
-  </si>
-  <si>
-    <t>63 Nova Drive</t>
-  </si>
-  <si>
-    <t>Elmira</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>607-341-1537</t>
-  </si>
-  <si>
-    <t>Rakel</t>
-  </si>
-  <si>
-    <t>Bartot</t>
-  </si>
-  <si>
-    <t>Hh6W5m</t>
-  </si>
-  <si>
-    <t>03 Cambridge Way</t>
-  </si>
-  <si>
-    <t>Richmond</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>804-805-8334</t>
-  </si>
-  <si>
-    <t>Casi</t>
-  </si>
-  <si>
-    <t>Terram</t>
-  </si>
-  <si>
-    <t>6KxfV20dnhAI</t>
-  </si>
-  <si>
-    <t>9 Florence Circle</t>
-  </si>
-  <si>
-    <t>Fullerton</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>714-220-2718</t>
-  </si>
-  <si>
-    <t>Erinna</t>
-  </si>
-  <si>
-    <t>Luckhurst</t>
-  </si>
-  <si>
-    <t>gu4QcS9El1Zf</t>
-  </si>
-  <si>
-    <t>6 Dryden Point</t>
-  </si>
-  <si>
-    <t>Tallahassee</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>850-826-7869</t>
-  </si>
-  <si>
-    <t>Darnall</t>
-  </si>
-  <si>
-    <t>Screech</t>
-  </si>
-  <si>
-    <t>zDm8CSBNl</t>
-  </si>
-  <si>
-    <t>16 Oxford Junction</t>
-  </si>
-  <si>
-    <t>504-339-3107</t>
+    <t>$26.01</t>
   </si>
 </sst>
 </file>
@@ -360,7 +348,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -400,7 +388,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,14 +705,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E752E530-4C12-4F61-B562-BFFFB21CE8A8}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -752,10 +744,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -768,9 +760,6 @@
       </c>
       <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -781,7 +770,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -792,19 +781,16 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -814,9 +800,6 @@
       </c>
       <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -827,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -838,19 +821,16 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -860,9 +840,6 @@
       </c>
       <c r="F6" t="s">
         <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -876,306 +853,306 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83099366-BCE8-424A-AA92-6E84CAADFD97}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G2" s="2">
         <v>23121</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2">
         <v>32123</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G4" s="2">
         <v>84199</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G5" s="2">
         <v>15215</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G6" s="2">
         <v>36616</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G7" s="2">
         <v>14905</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G8" s="2">
         <v>23228</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G9" s="2">
         <v>92835</v>
       </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G10" s="2">
         <v>32304</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G11" s="2">
         <v>70142</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>